<commit_message>
Fixed happy path test.
</commit_message>
<xml_diff>
--- a/test/support/fixtures/xlsx/valid.xlsx
+++ b/test/support/fixtures/xlsx/valid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmaddox/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75757726-C26E-8840-A27B-AA0E28E9D658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0D18D1-EDBF-924B-8000-3099B1AD3CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{89E0CC38-388B-4A33-B61B-82A90C1A9AB8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Notes</t>
   </si>
@@ -48,18 +48,6 @@
   </si>
   <si>
     <t>Wellington</t>
-  </si>
-  <si>
-    <t>Assembly</t>
-  </si>
-  <si>
-    <t>Sullivan Square</t>
-  </si>
-  <si>
-    <t>Community College</t>
-  </si>
-  <si>
-    <t>North Station</t>
   </si>
   <si>
     <t>Stop Name</t>
@@ -480,7 +468,9 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -491,10 +481,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -526,36 +516,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>28743</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>29002</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>9070028</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>9070026</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -583,10 +557,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -598,10 +572,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -609,59 +583,31 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>9070026</v>
+        <v>5271</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>9070029</v>
+        <v>5072</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>29002</v>
+        <v>9328</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>28742</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5271</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2">
-        <v>5072</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2">
-        <v>9328</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -680,15 +626,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAB132A750142542B3926DCF31A13A3D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="efe259cd95b139b8a430fcab0a53d8ae">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0db2d361-8471-4f04-ae28-f5b2bb432068" xmlns:ns3="9ac8c65e-24cc-4907-9a10-66b1170b57fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="443ac76d90ee1648d07c0937ebde1acd" ns2:_="" ns3:_="">
     <xsd:import namespace="0db2d361-8471-4f04-ae28-f5b2bb432068"/>
@@ -917,6 +854,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C457723D-4526-420E-9AFF-DF32F9694D3B}">
   <ds:schemaRefs>
@@ -929,14 +875,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{230200EC-77C1-4FD2-9CAB-0EDB6EEE0881}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -953,4 +891,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA46E352-1983-4CFE-ABFE-F18FB5E48C0B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>